<commit_message>
Auto push at 07:26:42
</commit_message>
<xml_diff>
--- a/semester 3/ais/accounting/problem solves/prev_questions.xlsx
+++ b/semester 3/ais/accounting/problem solves/prev_questions.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="temp" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="4b" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="adjusted entry" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="2015" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="temp_2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="4b" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="adjusted entry" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="2015" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="78">
   <si>
     <t xml:space="preserve">P1-1B</t>
   </si>
@@ -385,7 +386,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -462,19 +463,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1134,8 +1131,8 @@
   </sheetPr>
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1242,15 +1239,18 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="n">
-        <v>55000</v>
+        <v>57000</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="E4" s="8" t="n">
+        <v>32500</v>
+      </c>
       <c r="F4" s="5"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="n">
-        <v>55000</v>
+        <f aca="false">B4+E4</f>
+        <v>89500</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -1261,7 +1261,7 @@
       <c r="N4" s="5"/>
       <c r="O4" s="8" t="n">
         <f aca="false">SUM(B4:B1000)</f>
-        <v>67700</v>
+        <v>57000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,14 +1270,10 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
-      <c r="D5" s="8" t="n">
-        <v>10600</v>
-      </c>
+      <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="8" t="n">
-        <v>10600</v>
-      </c>
+      <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -1288,27 +1284,21 @@
       <c r="N5" s="5"/>
       <c r="O5" s="8" t="n">
         <f aca="false">SUM(C4:C1000)</f>
-        <v>800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="n">
-        <v>11500</v>
-      </c>
-      <c r="C6" s="8" t="n">
-        <v>2000</v>
-      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="5"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="8" t="n">
-        <v>13500</v>
-      </c>
+      <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="M6" s="5" t="s">
@@ -1317,7 +1307,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="8" t="n">
         <f aca="false">SUM(D4:D1000)</f>
-        <v>10600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1329,14 +1319,10 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="8" t="n">
-        <v>2500</v>
-      </c>
+      <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
-      <c r="J7" s="8" t="n">
-        <v>-2500</v>
-      </c>
+      <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="M7" s="5" t="s">
         <v>17</v>
@@ -1344,19 +1330,15 @@
       <c r="N7" s="5"/>
       <c r="O7" s="8" t="n">
         <f aca="false">SUM(E4:E1000)</f>
-        <v>0</v>
+        <v>32500</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="n">
-        <v>1200</v>
-      </c>
-      <c r="C8" s="8" t="n">
-        <v>-1200</v>
-      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="5"/>
@@ -1371,7 +1353,7 @@
       <c r="N8" s="10"/>
       <c r="O8" s="11" t="n">
         <f aca="false">SUM(O4:O7)</f>
-        <v>79100</v>
+        <v>89500</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1448,7 +1430,7 @@
       </c>
       <c r="O12" s="8" t="n">
         <f aca="false">SUM(G4:G1000)</f>
-        <v>13100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1477,7 +1459,7 @@
       </c>
       <c r="O14" s="8" t="n">
         <f aca="false">SUM(H4:H1000)</f>
-        <v>55000</v>
+        <v>89500</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,7 +1469,7 @@
       </c>
       <c r="O15" s="8" t="n">
         <f aca="false">SUM(I4:K1000)</f>
-        <v>11000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,7 +1479,7 @@
       <c r="N16" s="10"/>
       <c r="O16" s="11" t="n">
         <f aca="false">O12+O14+O15</f>
-        <v>79100</v>
+        <v>89500</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1529,7 +1511,7 @@
       </c>
       <c r="N22" s="8" t="n">
         <f aca="false">SUM(I4:I1000)</f>
-        <v>13500</v>
+        <v>0</v>
       </c>
       <c r="O22" s="3"/>
     </row>
@@ -1539,7 +1521,7 @@
       </c>
       <c r="N23" s="8" t="n">
         <f aca="false">SUM(J4:J1000)</f>
-        <v>-2500</v>
+        <v>0</v>
       </c>
       <c r="O23" s="3"/>
     </row>
@@ -1549,7 +1531,7 @@
       </c>
       <c r="N24" s="11" t="n">
         <f aca="false">N22+N23</f>
-        <v>11000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1565,7 +1547,7 @@
       </c>
       <c r="N28" s="8" t="n">
         <f aca="false">N24</f>
-        <v>11000</v>
+        <v>0</v>
       </c>
       <c r="O28" s="3"/>
     </row>
@@ -1585,7 +1567,7 @@
       </c>
       <c r="N30" s="11" t="n">
         <f aca="false">N28+N29</f>
-        <v>11000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1624,6 +1606,498 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:P30"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="2.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="22.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="19.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.81"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>55000</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8" t="n">
+        <v>55000</v>
+      </c>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="M4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="8" t="n">
+        <f aca="false">SUM(B4:B1000)</f>
+        <v>67700</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="n">
+        <v>10600</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="8" t="n">
+        <v>10600</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="M5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="8" t="n">
+        <f aca="false">SUM(C4:C1000)</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8" t="n">
+        <v>11500</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8" t="n">
+        <v>13500</v>
+      </c>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="M6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="O6" s="8" t="n">
+        <f aca="false">SUM(D4:D1000)</f>
+        <v>10600</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="8" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8" t="n">
+        <v>-2500</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="M7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="5"/>
+      <c r="O7" s="8" t="n">
+        <f aca="false">SUM(E4:E1000)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8" t="n">
+        <v>1200</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>-1200</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="M8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="10"/>
+      <c r="O8" s="11" t="n">
+        <f aca="false">SUM(O4:O7)</f>
+        <v>79100</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="M10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="M11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" s="9"/>
+      <c r="O11" s="12"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="N12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="8" t="n">
+        <f aca="false">SUM(G4:G1000)</f>
+        <v>13100</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="M13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" s="9"/>
+      <c r="O13" s="12"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <f aca="false">SUM(H4:H1000)</f>
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M15" s="14"/>
+      <c r="N15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <f aca="false">SUM(I4:K1000)</f>
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="10"/>
+      <c r="O16" s="11" t="n">
+        <f aca="false">O12+O14+O15</f>
+        <v>79100</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" s="15" t="str">
+        <f aca="false">IF(O8=O16,"No error, it seems!","Error exists!")</f>
+        <v>No error, it seems!</v>
+      </c>
+      <c r="O18" s="15"/>
+      <c r="P18" s="12"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <f aca="false">SUM(I4:I1000)</f>
+        <v>13500</v>
+      </c>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M23" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <f aca="false">SUM(J4:J1000)</f>
+        <v>-2500</v>
+      </c>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M24" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N24" s="11" t="n">
+        <f aca="false">N22+N23</f>
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N28" s="8" t="n">
+        <f aca="false">N24</f>
+        <v>11000</v>
+      </c>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N29" s="8" t="n">
+        <f aca="false">SUM(K4:K1000)</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M30" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="N30" s="11" t="n">
+        <f aca="false">N28+N29</f>
+        <v>11000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:F13"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M26:O26"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1992,531 +2466,531 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="15.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="12" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="12" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>58</v>
       </c>
       <c r="D4" s="19"/>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="21" t="n">
+      <c r="C6" s="20" t="n">
         <v>5300</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="F6" s="0" t="s">
+      <c r="D6" s="20"/>
+      <c r="F6" s="12" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="21" t="n">
+      <c r="C7" s="20" t="n">
         <v>10800</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="G7" s="0" t="str">
+      <c r="D7" s="20"/>
+      <c r="G7" s="12" t="str">
         <f aca="false">A6</f>
         <v>Cash</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7" s="12" t="n">
         <f aca="false">C6</f>
         <v>5300</v>
       </c>
-      <c r="K7" s="22" t="n">
+      <c r="K7" s="21" t="n">
         <f aca="false">SUM(J7:J12)</f>
         <v>41000</v>
       </c>
-      <c r="L7" s="22"/>
+      <c r="L7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="21" t="n">
+      <c r="C8" s="20" t="n">
         <v>1500</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="G8" s="0" t="str">
+      <c r="D8" s="20"/>
+      <c r="G8" s="12" t="str">
         <f aca="false">A7</f>
         <v>Accounts Receivable</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8" s="12" t="n">
         <f aca="false">C7</f>
         <v>10800</v>
       </c>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="21" t="n">
+      <c r="C9" s="20" t="n">
         <v>2000</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="G9" s="0" t="str">
+      <c r="D9" s="20"/>
+      <c r="G9" s="12" t="str">
         <f aca="false">A8</f>
         <v>Supplies</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9" s="12" t="n">
         <f aca="false">C8</f>
         <v>1500</v>
       </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="21" t="n">
+      <c r="C10" s="20" t="n">
         <v>27000</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="G10" s="0" t="str">
+      <c r="D10" s="20"/>
+      <c r="G10" s="12" t="str">
         <f aca="false">A9</f>
         <v>Prepaid Insurance</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10" s="12" t="n">
         <f aca="false">C9</f>
         <v>2000</v>
       </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21" t="n">
+      <c r="C11" s="20"/>
+      <c r="D11" s="20" t="n">
         <v>5600</v>
       </c>
-      <c r="G11" s="0" t="str">
+      <c r="G11" s="12" t="str">
         <f aca="false">A10</f>
         <v>Equipment</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J11" s="12" t="n">
         <f aca="false">C10</f>
         <v>27000</v>
       </c>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21" t="n">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20" t="n">
         <v>15000</v>
       </c>
-      <c r="G12" s="0" t="str">
+      <c r="G12" s="12" t="str">
         <f aca="false">A11</f>
         <v>Accumulated Depreciation</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J12" s="12" t="n">
         <f aca="false">-D11</f>
         <v>-5600</v>
       </c>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21" t="n">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20" t="n">
         <v>6100</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21" t="n">
+      <c r="C14" s="20"/>
+      <c r="D14" s="20" t="n">
         <v>2400</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21" t="n">
+      <c r="C15" s="20"/>
+      <c r="D15" s="20" t="n">
         <v>600</v>
       </c>
-      <c r="G15" s="0" t="str">
+      <c r="G15" s="12" t="str">
         <f aca="false">A12</f>
         <v>Notes Payable</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="J15" s="12" t="n">
         <f aca="false">D12</f>
         <v>15000</v>
       </c>
-      <c r="K15" s="22" t="n">
+      <c r="K15" s="21" t="n">
         <f aca="false">SUM(J15:J18)</f>
         <v>24100</v>
       </c>
-      <c r="L15" s="22" t="n">
+      <c r="L15" s="21" t="n">
         <f aca="false">K25</f>
         <v>41000</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21" t="n">
+      <c r="C16" s="20"/>
+      <c r="D16" s="20" t="n">
         <v>13000</v>
       </c>
-      <c r="G16" s="0" t="str">
+      <c r="G16" s="12" t="str">
         <f aca="false">A13</f>
         <v>Accounts Payable</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="J16" s="12" t="n">
         <f aca="false">D13</f>
         <v>6100</v>
       </c>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="21" t="n">
+      <c r="C17" s="20" t="n">
         <v>7000</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="G17" s="0" t="str">
+      <c r="D17" s="20"/>
+      <c r="G17" s="12" t="str">
         <f aca="false">A14</f>
         <v>Salaries and Wages Payable</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="J17" s="12" t="n">
         <f aca="false">D14</f>
         <v>2400</v>
       </c>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21" t="n">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20" t="n">
         <v>61000</v>
       </c>
-      <c r="G18" s="0" t="str">
+      <c r="G18" s="12" t="str">
         <f aca="false">A15</f>
         <v>Interest Payable</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="J18" s="12" t="n">
         <f aca="false">D15</f>
         <v>600</v>
       </c>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="21" t="n">
+      <c r="C19" s="20" t="n">
         <v>8400</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="L19" s="22"/>
+      <c r="D19" s="20"/>
+      <c r="L19" s="21"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="21" t="n">
+      <c r="C20" s="20" t="n">
         <v>4000</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="L20" s="22"/>
+      <c r="D20" s="20"/>
+      <c r="L20" s="21"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="21" t="n">
+      <c r="C21" s="20" t="n">
         <v>5600</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="F21" s="0" t="s">
+      <c r="D21" s="20"/>
+      <c r="F21" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="L21" s="22"/>
+      <c r="L21" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="21" t="n">
+      <c r="C22" s="20" t="n">
         <v>3500</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="G22" s="0" t="str">
+      <c r="D22" s="20"/>
+      <c r="G22" s="12" t="str">
         <f aca="false">A16</f>
         <v>Owner’s Capital</v>
       </c>
-      <c r="J22" s="0" t="n">
+      <c r="J22" s="12" t="n">
         <f aca="false">D16</f>
         <v>13000</v>
       </c>
-      <c r="K22" s="22" t="n">
+      <c r="K22" s="21" t="n">
         <f aca="false">SUM(J22:J23)</f>
         <v>16900</v>
       </c>
-      <c r="L22" s="22"/>
+      <c r="L22" s="21"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="21" t="n">
+      <c r="C23" s="20" t="n">
         <v>28000</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="G23" s="0" t="str">
+      <c r="D23" s="20"/>
+      <c r="G23" s="12" t="str">
         <f aca="false">F33</f>
         <v>Retained Earning, Dec</v>
       </c>
-      <c r="J23" s="0" t="n">
+      <c r="J23" s="12" t="n">
         <f aca="false">I33</f>
         <v>3900</v>
       </c>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="21" t="n">
+      <c r="C24" s="20" t="n">
         <v>600</v>
       </c>
-      <c r="D24" s="21"/>
+      <c r="D24" s="20"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="20" t="n">
+      <c r="C25" s="16" t="n">
         <f aca="false">SUM(C6:C24)</f>
         <v>103700</v>
       </c>
-      <c r="D25" s="20" t="n">
+      <c r="D25" s="16" t="n">
         <f aca="false">SUM(D6:D24)</f>
         <v>103700</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20" t="n">
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16" t="n">
         <f aca="false">K15+K22</f>
         <v>41000</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="16" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="12" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="str">
+      <c r="B30" s="12" t="str">
         <f aca="false">A18</f>
         <v>Service Revenue</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="12" t="n">
         <f aca="false">D18</f>
         <v>61000</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="F30" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="I30" s="0" t="n">
+      <c r="I30" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20" t="n">
+      <c r="C31" s="16"/>
+      <c r="D31" s="16" t="n">
         <f aca="false">D30</f>
         <v>61000</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="F31" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="I31" s="0" t="n">
+      <c r="I31" s="12" t="n">
         <f aca="false">D42</f>
         <v>10900</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F32" s="0" t="s">
+      <c r="F32" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I32" s="0" t="n">
+      <c r="I32" s="12" t="n">
         <v>7000</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20" t="n">
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16" t="n">
         <f aca="false">I31-I32</f>
         <v>3900</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="str">
+      <c r="B34" s="12" t="str">
         <f aca="false">A19</f>
         <v>Advertising Expense</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="12" t="n">
         <f aca="false">C19</f>
         <v>8400</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="str">
+      <c r="B35" s="12" t="str">
         <f aca="false">A20</f>
         <v>Supplies Expense</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="12" t="n">
         <f aca="false">C20</f>
         <v>4000</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="str">
+      <c r="B36" s="12" t="str">
         <f aca="false">A21</f>
         <v>Depreciation Expense</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="12" t="n">
         <f aca="false">C21</f>
         <v>5600</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="str">
+      <c r="B37" s="12" t="str">
         <f aca="false">A22</f>
         <v>Insurance Expense</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37" s="12" t="n">
         <f aca="false">C22</f>
         <v>3500</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="str">
+      <c r="B38" s="12" t="str">
         <f aca="false">A23</f>
         <v>Salaries and Wages Expense</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D38" s="12" t="n">
         <f aca="false">C23</f>
         <v>28000</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="str">
+      <c r="B39" s="12" t="str">
         <f aca="false">A24</f>
         <v>Interest Expense</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39" s="12" t="n">
         <f aca="false">C24</f>
         <v>600</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20" t="n">
+      <c r="C40" s="16"/>
+      <c r="D40" s="16" t="n">
         <f aca="false">SUM(D34:D39)</f>
         <v>50100</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D42" s="0" t="n">
+      <c r="D42" s="12" t="n">
         <f aca="false">D31-D40</f>
         <v>10900</v>
       </c>

</xml_diff>